<commit_message>
Versiones finales post corrección de estilo
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado05/guion01/SolicitudGrafica_LE_05_01_CO.xlsx
+++ b/fuentes/contenidos/grado05/guion01/SolicitudGrafica_LE_05_01_CO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14200" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Solicitud gráfica" sheetId="1" r:id="rId1"/>
@@ -1490,6 +1490,24 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1546,24 +1564,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="51">
@@ -2315,7 +2315,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I19" sqref="I19"/>
+      <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -2336,7 +2336,7 @@
     <col min="14" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="16.25" thickBot="1">
+    <row r="1" spans="1:16" ht="16" thickBot="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -2348,15 +2348,15 @@
       <c r="J1" s="16"/>
       <c r="K1" s="16"/>
     </row>
-    <row r="2" spans="1:16" ht="15.75">
+    <row r="2" spans="1:16" ht="15">
       <c r="A2" s="1"/>
       <c r="B2" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C2" s="105" t="s">
+      <c r="C2" s="87" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="106"/>
+      <c r="D2" s="88"/>
       <c r="F2" s="80" t="s">
         <v>0</v>
       </c>
@@ -2365,30 +2365,32 @@
       <c r="I2" s="56"/>
       <c r="J2" s="16"/>
     </row>
-    <row r="3" spans="1:16" ht="15.75">
+    <row r="3" spans="1:16" ht="15">
       <c r="A3" s="1"/>
       <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="107">
+      <c r="C3" s="89">
         <v>5</v>
       </c>
-      <c r="D3" s="108"/>
-      <c r="F3" s="82"/>
+      <c r="D3" s="90"/>
+      <c r="F3" s="82">
+        <v>42073</v>
+      </c>
       <c r="G3" s="83"/>
       <c r="H3" s="56"/>
       <c r="I3" s="56"/>
       <c r="J3" s="16"/>
     </row>
-    <row r="4" spans="1:16" ht="15.75">
+    <row r="4" spans="1:16" ht="15">
       <c r="A4" s="1"/>
       <c r="B4" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="107" t="s">
+      <c r="C4" s="89" t="s">
         <v>145</v>
       </c>
-      <c r="D4" s="108"/>
+      <c r="D4" s="90"/>
       <c r="E4" s="5"/>
       <c r="F4" s="55" t="s">
         <v>55</v>
@@ -2401,15 +2403,15 @@
       <c r="J4" s="16"/>
       <c r="K4" s="16"/>
     </row>
-    <row r="5" spans="1:16" ht="16.25" thickBot="1">
+    <row r="5" spans="1:16" ht="16" thickBot="1">
       <c r="A5" s="1"/>
       <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="109" t="s">
+      <c r="C5" s="91" t="s">
         <v>146</v>
       </c>
-      <c r="D5" s="110"/>
+      <c r="D5" s="92"/>
       <c r="E5" s="5"/>
       <c r="F5" s="53" t="str">
         <f>IF(G4="Recurso","Motor del recurso","")</f>
@@ -2421,7 +2423,7 @@
       <c r="J5" s="16"/>
       <c r="K5" s="16"/>
     </row>
-    <row r="6" spans="1:16" ht="16.25" thickBot="1">
+    <row r="6" spans="1:16" ht="16" thickBot="1">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -2452,7 +2454,7 @@
       <c r="J7" s="16"/>
       <c r="K7" s="16"/>
     </row>
-    <row r="8" spans="1:16" s="9" customFormat="1" ht="16.25" thickBot="1">
+    <row r="8" spans="1:16" s="9" customFormat="1" ht="16" thickBot="1">
       <c r="A8" s="10"/>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
@@ -2737,7 +2739,7 @@
     </row>
     <row r="16" spans="1:16" s="12" customFormat="1">
       <c r="A16" s="13" t="str">
-        <f t="shared" ref="A12:A30" si="3">IF(OR(B16&lt;&gt;"",J16&lt;&gt;""),CONCATENATE(LEFT(A15,3),IF(MID(A15,4,2)+1&lt;10,CONCATENATE("0",MID(A15,4,2)+1))),"")</f>
+        <f t="shared" ref="A16:A30" si="3">IF(OR(B16&lt;&gt;"",J16&lt;&gt;""),CONCATENATE(LEFT(A15,3),IF(MID(A15,4,2)+1&lt;10,CONCATENATE("0",MID(A15,4,2)+1))),"")</f>
         <v/>
       </c>
       <c r="B16" s="28"/>
@@ -2766,7 +2768,7 @@
       <c r="J16" s="34"/>
       <c r="K16" s="37"/>
     </row>
-    <row r="17" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="17" spans="1:11" s="12" customFormat="1">
       <c r="A17" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -2797,7 +2799,7 @@
       <c r="J17" s="21"/>
       <c r="K17" s="21"/>
     </row>
-    <row r="18" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="18" spans="1:11" s="12" customFormat="1">
       <c r="A18" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -2828,7 +2830,7 @@
       <c r="J18" s="21"/>
       <c r="K18" s="21"/>
     </row>
-    <row r="19" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="19" spans="1:11" s="12" customFormat="1">
       <c r="A19" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -2859,7 +2861,7 @@
       <c r="J19" s="34"/>
       <c r="K19" s="37"/>
     </row>
-    <row r="20" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="20" spans="1:11" s="12" customFormat="1">
       <c r="A20" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -2890,7 +2892,7 @@
       <c r="J20" s="19"/>
       <c r="K20" s="21"/>
     </row>
-    <row r="21" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="21" spans="1:11" s="12" customFormat="1">
       <c r="A21" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -2921,7 +2923,7 @@
       <c r="J21" s="21"/>
       <c r="K21" s="21"/>
     </row>
-    <row r="22" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="22" spans="1:11" s="12" customFormat="1">
       <c r="A22" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -2952,7 +2954,7 @@
       <c r="J22" s="14"/>
       <c r="K22" s="20"/>
     </row>
-    <row r="23" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="23" spans="1:11" s="12" customFormat="1">
       <c r="A23" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -2980,7 +2982,7 @@
       <c r="J23" s="19"/>
       <c r="K23" s="19"/>
     </row>
-    <row r="24" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="24" spans="1:11" s="12" customFormat="1">
       <c r="A24" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3008,7 +3010,7 @@
       <c r="J24" s="14"/>
       <c r="K24" s="15"/>
     </row>
-    <row r="25" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="25" spans="1:11" s="12" customFormat="1">
       <c r="A25" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3036,7 +3038,7 @@
       <c r="J25" s="14"/>
       <c r="K25" s="19"/>
     </row>
-    <row r="26" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="26" spans="1:11" s="12" customFormat="1">
       <c r="A26" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3064,7 +3066,7 @@
       <c r="J26" s="14"/>
       <c r="K26" s="19"/>
     </row>
-    <row r="27" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="27" spans="1:11" s="12" customFormat="1">
       <c r="A27" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3092,7 +3094,7 @@
       <c r="J27" s="19"/>
       <c r="K27" s="19"/>
     </row>
-    <row r="28" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="28" spans="1:11" s="12" customFormat="1">
       <c r="A28" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3120,7 +3122,7 @@
       <c r="J28" s="19"/>
       <c r="K28" s="19"/>
     </row>
-    <row r="29" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="29" spans="1:11" s="12" customFormat="1">
       <c r="A29" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3148,7 +3150,7 @@
       <c r="J29" s="19"/>
       <c r="K29" s="19"/>
     </row>
-    <row r="30" spans="1:11" s="12" customFormat="1" ht="15">
+    <row r="30" spans="1:11" s="12" customFormat="1">
       <c r="A30" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5202,38 +5204,38 @@
     <col min="12" max="16384" width="10.83203125" style="38"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="16.25" thickBot="1">
-      <c r="A1" s="89" t="s">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
+      <c r="A1" s="95" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="90"/>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="91"/>
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="97"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="46" t="s">
         <v>42</v>
       </c>
       <c r="B2" s="47"/>
-      <c r="C2" s="92" t="s">
+      <c r="C2" s="98" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="93"/>
-      <c r="E2" s="94"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="100"/>
       <c r="F2" s="48"/>
     </row>
-    <row r="3" spans="1:11" ht="63.25">
+    <row r="3" spans="1:11" ht="60">
       <c r="A3" s="49" t="s">
         <v>43</v>
       </c>
       <c r="B3" s="47"/>
-      <c r="C3" s="98" t="s">
+      <c r="C3" s="104" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="99"/>
-      <c r="E3" s="100"/>
+      <c r="D3" s="105"/>
+      <c r="E3" s="106"/>
       <c r="F3" s="48"/>
       <c r="H3" s="38" t="s">
         <v>18</v>
@@ -5248,7 +5250,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="31.75">
+    <row r="4" spans="1:11" ht="30">
       <c r="A4" s="46" t="s">
         <v>44</v>
       </c>
@@ -5276,7 +5278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="79.5" thickBot="1">
+    <row r="5" spans="1:11" ht="76" thickBot="1">
       <c r="A5" s="49" t="s">
         <v>45</v>
       </c>
@@ -5284,11 +5286,11 @@
       <c r="C5" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="101" t="str">
+      <c r="D5" s="107" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_CO")</f>
         <v>LE_07_04_CO</v>
       </c>
-      <c r="E5" s="102"/>
+      <c r="E5" s="108"/>
       <c r="F5" s="48"/>
       <c r="H5" s="38" t="s">
         <v>22</v>
@@ -5303,7 +5305,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="32" thickBot="1">
+    <row r="6" spans="1:11" ht="31" thickBot="1">
       <c r="A6" s="46" t="s">
         <v>10</v>
       </c>
@@ -5325,7 +5327,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="32" thickBot="1">
+    <row r="7" spans="1:11" ht="46" thickBot="1">
       <c r="A7" s="49" t="s">
         <v>11</v>
       </c>
@@ -5333,12 +5335,12 @@
       <c r="C7" s="78" t="s">
         <v>127</v>
       </c>
-      <c r="D7" s="87" t="str">
+      <c r="D7" s="93" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D5,".xls")</f>
         <v>SolicitudGrafica_LE_07_04_CO.xls</v>
       </c>
-      <c r="E7" s="87"/>
-      <c r="F7" s="88"/>
+      <c r="E7" s="93"/>
+      <c r="F7" s="94"/>
       <c r="H7" s="38" t="s">
         <v>24</v>
       </c>
@@ -5352,7 +5354,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="47.5">
+    <row r="8" spans="1:11" ht="45">
       <c r="A8" s="49" t="s">
         <v>53</v>
       </c>
@@ -5371,7 +5373,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="47.5">
+    <row r="9" spans="1:11" ht="45">
       <c r="A9" s="49" t="s">
         <v>12</v>
       </c>
@@ -5390,7 +5392,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="32" thickBot="1">
+    <row r="10" spans="1:11" ht="31" thickBot="1">
       <c r="A10" s="50" t="s">
         <v>36</v>
       </c>
@@ -5420,7 +5422,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="16.25" thickBot="1">
+    <row r="12" spans="1:11" ht="16" thickBot="1">
       <c r="I12" s="38" t="s">
         <v>37</v>
       </c>
@@ -5432,14 +5434,14 @@
       </c>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="89" t="s">
+      <c r="A13" s="95" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="90"/>
-      <c r="C13" s="90"/>
-      <c r="D13" s="90"/>
-      <c r="E13" s="90"/>
-      <c r="F13" s="91"/>
+      <c r="B13" s="96"/>
+      <c r="C13" s="96"/>
+      <c r="D13" s="96"/>
+      <c r="E13" s="96"/>
+      <c r="F13" s="97"/>
       <c r="I13" s="38" t="s">
         <v>33</v>
       </c>
@@ -5450,7 +5452,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="16.25" thickBot="1">
+    <row r="14" spans="1:11" ht="16" thickBot="1">
       <c r="A14" s="49"/>
       <c r="B14" s="47"/>
       <c r="C14" s="47"/>
@@ -5472,12 +5474,12 @@
         <v>46</v>
       </c>
       <c r="B15" s="47"/>
-      <c r="C15" s="92" t="s">
+      <c r="C15" s="98" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="93"/>
-      <c r="E15" s="93"/>
-      <c r="F15" s="94"/>
+      <c r="D15" s="99"/>
+      <c r="E15" s="99"/>
+      <c r="F15" s="100"/>
       <c r="J15" s="38">
         <v>12</v>
       </c>
@@ -5517,12 +5519,12 @@
       <c r="C17" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="95" t="str">
+      <c r="D17" s="101" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_",K45)</f>
         <v>LE_07_04_REC10</v>
       </c>
-      <c r="E17" s="96"/>
-      <c r="F17" s="97"/>
+      <c r="E17" s="102"/>
+      <c r="F17" s="103"/>
       <c r="J17" s="38">
         <v>14</v>
       </c>
@@ -5530,7 +5532,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="79.5" thickBot="1">
+    <row r="18" spans="1:11" ht="76" thickBot="1">
       <c r="A18" s="49" t="s">
         <v>48</v>
       </c>
@@ -5538,12 +5540,12 @@
       <c r="C18" s="78" t="s">
         <v>128</v>
       </c>
-      <c r="D18" s="87" t="str">
+      <c r="D18" s="93" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D17,".xls")</f>
         <v>SolicitudGrafica_LE_07_04_REC10.xls</v>
       </c>
-      <c r="E18" s="87"/>
-      <c r="F18" s="88"/>
+      <c r="E18" s="93"/>
+      <c r="F18" s="94"/>
       <c r="J18" s="38">
         <v>15</v>
       </c>
@@ -5570,7 +5572,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="63.75" thickBot="1">
+    <row r="20" spans="1:11" ht="61" thickBot="1">
       <c r="A20" s="50" t="s">
         <v>51</v>
       </c>
@@ -5947,41 +5949,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="103" t="s">
+      <c r="A1" s="109" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="103" t="s">
+      <c r="B1" s="109" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="103" t="s">
+      <c r="C1" s="109" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="103" t="s">
+      <c r="D1" s="109" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="103" t="s">
+      <c r="E1" s="109" t="s">
         <v>65</v>
       </c>
-      <c r="F1" s="103" t="s">
+      <c r="F1" s="109" t="s">
         <v>66</v>
       </c>
-      <c r="G1" s="103" t="s">
+      <c r="G1" s="109" t="s">
         <v>67</v>
       </c>
-      <c r="H1" s="104" t="s">
+      <c r="H1" s="110" t="s">
         <v>68</v>
       </c>
-      <c r="I1" s="104"/>
-      <c r="J1" s="104"/>
+      <c r="I1" s="110"/>
+      <c r="J1" s="110"/>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="103"/>
-      <c r="B2" s="103"/>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
+      <c r="A2" s="109"/>
+      <c r="B2" s="109"/>
+      <c r="C2" s="109"/>
+      <c r="D2" s="109"/>
+      <c r="E2" s="109"/>
+      <c r="F2" s="109"/>
+      <c r="G2" s="109"/>
       <c r="H2" s="57" t="s">
         <v>65</v>
       </c>
@@ -6104,7 +6106,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="59" customFormat="1" ht="26.5">
+    <row r="7" spans="1:11" s="59" customFormat="1" ht="28">
       <c r="A7" s="60" t="s">
         <v>80</v>
       </c>
@@ -6132,7 +6134,7 @@
       </c>
       <c r="J7" s="60"/>
     </row>
-    <row r="8" spans="1:11" s="59" customFormat="1">
+    <row r="8" spans="1:11" s="59" customFormat="1" ht="28">
       <c r="A8" s="60" t="s">
         <v>82</v>
       </c>
@@ -6214,7 +6216,7 @@
       </c>
       <c r="J10" s="60"/>
     </row>
-    <row r="11" spans="1:11" s="59" customFormat="1" ht="26.5">
+    <row r="11" spans="1:11" s="59" customFormat="1" ht="28">
       <c r="A11" s="60" t="s">
         <v>89</v>
       </c>
@@ -6270,7 +6272,7 @@
       </c>
       <c r="J12" s="60"/>
     </row>
-    <row r="13" spans="1:11" ht="63.25">
+    <row r="13" spans="1:11" ht="60">
       <c r="A13" s="63" t="s">
         <v>93</v>
       </c>
@@ -6321,7 +6323,7 @@
       </c>
       <c r="J14" s="63"/>
     </row>
-    <row r="15" spans="1:11" ht="31.75">
+    <row r="15" spans="1:11" ht="30">
       <c r="A15" s="63" t="s">
         <v>99</v>
       </c>
@@ -6348,7 +6350,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="95">
+    <row r="16" spans="1:11" ht="90">
       <c r="A16" s="65" t="s">
         <v>103</v>
       </c>
@@ -6377,7 +6379,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="26.5">
+    <row r="17" spans="1:11" ht="28">
       <c r="A17" s="60" t="s">
         <v>106</v>
       </c>
@@ -6450,7 +6452,7 @@
       <c r="D23" s="74"/>
       <c r="E23" s="74"/>
     </row>
-    <row r="24" spans="1:11" ht="31.75">
+    <row r="24" spans="1:11" ht="30">
       <c r="A24" s="73" t="s">
         <v>116</v>
       </c>
@@ -6476,7 +6478,7 @@
       <c r="D25" s="74"/>
       <c r="E25" s="74"/>
     </row>
-    <row r="26" spans="1:11" ht="63.25">
+    <row r="26" spans="1:11" ht="60">
       <c r="A26" s="73" t="s">
         <v>118</v>
       </c>

</xml_diff>